<commit_message>
rewrote concept of lgbmf
</commit_message>
<xml_diff>
--- a/1_literature/0-literature-list.xlsx
+++ b/1_literature/0-literature-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\semester_3\manifold\manifold-lle\1_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B92F3B-5C8C-49C2-89FE-55BB0ABF36D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E4703E-6F2B-4136-9050-722C95E6C900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F98F86D9-6731-4315-91B3-50135AD40D0D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
   <si>
     <t>authors</t>
   </si>
@@ -364,6 +364,18 @@
   </si>
   <si>
     <t>eigenvalue problems, simple and good to follow</t>
+  </si>
+  <si>
+    <t>wu, wu</t>
+  </si>
+  <si>
+    <t>think globally, fit locally under the manifold setup. Asymptotic analysis of lle</t>
+  </si>
+  <si>
+    <t>lle, laplace-beltrami</t>
+  </si>
+  <si>
+    <t>lle not related to laplace-beltrami?!</t>
   </si>
 </sst>
 </file>
@@ -719,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C80217-AEA8-44B1-8036-614621D3A806}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,6 +1428,26 @@
         <v>108</v>
       </c>
     </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F8" xr:uid="{853C53E3-02E1-4899-8524-107A10212B6F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">

</xml_diff>

<commit_message>
refactored concept chapter acc to new learnings
</commit_message>
<xml_diff>
--- a/1_literature/0-literature-list.xlsx
+++ b/1_literature/0-literature-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wimme\Documents\1_uni\1_master\semester_3\manifold\manifold-lle\1_literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E4703E-6F2B-4136-9050-722C95E6C900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDFB1A0-0DB7-472A-B67E-158FF52535EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F98F86D9-6731-4315-91B3-50135AD40D0D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="116">
   <si>
     <t>authors</t>
   </si>
@@ -376,6 +376,15 @@
   </si>
   <si>
     <t>lle not related to laplace-beltrami?!</t>
+  </si>
+  <si>
+    <t>laplace-beltrami</t>
+  </si>
+  <si>
+    <t>theoretical foundation of using graph laplacian</t>
+  </si>
+  <si>
+    <t>towards a theoretical foundation of laplacian-based manifold methods</t>
   </si>
 </sst>
 </file>
@@ -731,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79C80217-AEA8-44B1-8036-614621D3A806}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,6 +1457,26 @@
         <v>112</v>
       </c>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2005</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F8" xr:uid="{853C53E3-02E1-4899-8524-107A10212B6F}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F32">

</xml_diff>